<commit_message>
Finish parameters for FlowDroid latest version
</commit_message>
<xml_diff>
--- a/ResessWelcome/515e684a672516a0d06fd3f769a69ffec1e6f9c5/attachments/FlowDroidManual.xlsx
+++ b/ResessWelcome/515e684a672516a0d06fd3f769a69ffec1e6f9c5/attachments/FlowDroidManual.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\eDocs\MASc\resess.github.io\ResessWelcome\515e684a672516a0d06fd3f769a69ffec1e6f9c5\attachments\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{2EE9E319-39A5-4CA7-A9BA-567637D4B747}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37CA4C59-9AFB-468A-A299-FA1D33283CF0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18870" windowHeight="7050" xr2:uid="{3B99BC71-4CF2-464B-9796-F55CDCCA280D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7335" windowHeight="7050" xr2:uid="{3B99BC71-4CF2-464B-9796-F55CDCCA280D}"/>
   </bookViews>
   <sheets>
     <sheet name="FD271" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FD271'!$A$1:$E$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'FD271'!$A$1:$F$45</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="164">
   <si>
     <t>Option</t>
   </si>
@@ -173,9 +173,6 @@
     <t>pathreconstructionmode</t>
   </si>
   <si>
-    <t>Use the specified mode for reconstructing taint propagation paths (NONE, FAST, PRECISE).</t>
-  </si>
-  <si>
     <t>implicit</t>
   </si>
   <si>
@@ -257,9 +254,6 @@
     <t>Outputs a file with information about which summaries are missing.</t>
   </si>
   <si>
-    <t>Use the specified taint wrapper algorithm (NONE, EASY, STUBDROID, MULTI). **Note: NONE: No taint wrapper, EASY: Use taint wrappers defined in *taintwrapperfile*, STUBDROID: Use definitions defined in *taintwrapperfile*, MULTI: Use multiple definition files defined in *taintwrapperfile*.**</t>
-  </si>
-  <si>
     <t>Definition file for the taint wrapper.</t>
   </si>
   <si>
@@ -272,12 +266,6 @@
     <t>Use a flow-insensitive alias analysis.</t>
   </si>
   <si>
-    <t>Write the discovered sources and sinks to the log output.</t>
-  </si>
-  <si>
-    <t>Limit the maximum number of threads to the given value.</t>
-  </si>
-  <si>
     <t>Analyze one Android component at a time.</t>
   </si>
   <si>
@@ -308,12 +296,6 @@
     <t>Do not purify the ICC results, i.e., do not remove simple flows that also have a corresponding ICC flow.</t>
   </si>
   <si>
-    <t>Callgraph algorithm to use (AUTO, CHA, VTA, RTA, SPARK, GEOM).</t>
-  </si>
-  <si>
-    <t>Mode for considerung layout controls as sources (NONE, PWD, ALL).</t>
-  </si>
-  <si>
     <t>Use the specified algorithm for computing result paths (CONTEXTSENSITIVE, CONTEXTINSENSITIVE, SOURCESONLY).</t>
   </si>
   <si>
@@ -323,22 +305,226 @@
     <t>Use the specified data flow solver (CONTEXTFLOWSENSITIVE, FLOWINSENSITIVE).</t>
   </si>
   <si>
-    <t>Use the specified aliasing algorithm (NONE, FLOWSENSITIVE, PTSBASED, LAZY).</t>
-  </si>
-  <si>
-    <t>Use the specified code elimination algorithm (NONE, PROPAGATECONSTS, REMOVECODE).</t>
-  </si>
-  <si>
-    <t>Use the specified mode for defining which callbacks introduce which sources (NONE, ALL, SOURCELIST).</t>
-  </si>
-  <si>
-    <t>Use the specified mode when processing implicit data flows (NONE, ARRAYONLY, ALL).</t>
-  </si>
-  <si>
-    <t>Use the specified mode when tracking static data flows (CONTEXTFLOWSENSITIVE, CONTEXTFLOWINSENSITIVE, NONE).</t>
-  </si>
-  <si>
     <t>Analyze the full frameworks together with the app without any optimizations.</t>
+  </si>
+  <si>
+    <t>Use the specified taint wrapper algorithm (NONE, EASY, STUBDROID, MULTI). **Note: NONE: No taint wrapper, EASY: Use taint wrappers defined in *taintwrapperfile*, STUBDROID: Use definitions defined in *taintwrapperfile*, MULTI: Use multiple definition files defined in *taintwrapperfile*, DEFAULT: Use StubDroid with internal summaries.**</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>-c args</t>
+  </si>
+  <si>
+    <t>-s args</t>
+  </si>
+  <si>
+    <t>-t args</t>
+  </si>
+  <si>
+    <t>-l args</t>
+  </si>
+  <si>
+    <t>-o args</t>
+  </si>
+  <si>
+    <t>-ac args</t>
+  </si>
+  <si>
+    <t>-si args</t>
+  </si>
+  <si>
+    <t>-md args</t>
+  </si>
+  <si>
+    <t>-im args</t>
+  </si>
+  <si>
+    <t>-aa args</t>
+  </si>
+  <si>
+    <t>-dt args</t>
+  </si>
+  <si>
+    <t>-ct args</t>
+  </si>
+  <si>
+    <t>-rt args</t>
+  </si>
+  <si>
+    <t>-ns</t>
+  </si>
+  <si>
+    <t>-nc</t>
+  </si>
+  <si>
+    <t>-ne</t>
+  </si>
+  <si>
+    <t>-nt</t>
+  </si>
+  <si>
+    <t>-r</t>
+  </si>
+  <si>
+    <t>-tw args</t>
+  </si>
+  <si>
+    <t>-nr</t>
+  </si>
+  <si>
+    <t>-af</t>
+  </si>
+  <si>
+    <t>-cp</t>
+  </si>
+  <si>
+    <t>-os</t>
+  </si>
+  <si>
+    <t>-ot</t>
+  </si>
+  <si>
+    <t>-sp</t>
+  </si>
+  <si>
+    <t>-ls</t>
+  </si>
+  <si>
+    <t>-d</t>
+  </si>
+  <si>
+    <t>-ps</t>
+  </si>
+  <si>
+    <t>-np</t>
+  </si>
+  <si>
+    <t>-ff</t>
+  </si>
+  <si>
+    <t>-sa</t>
+  </si>
+  <si>
+    <t>-mt args</t>
+  </si>
+  <si>
+    <t>-al args</t>
+  </si>
+  <si>
+    <t>-mc args</t>
+  </si>
+  <si>
+    <t>-cg args</t>
+  </si>
+  <si>
+    <t>-pa args</t>
+  </si>
+  <si>
+    <t>-ca args</t>
+  </si>
+  <si>
+    <t>-ds args</t>
+  </si>
+  <si>
+    <t>-ce args</t>
+  </si>
+  <si>
+    <t>-cs args</t>
+  </si>
+  <si>
+    <t>-pr args</t>
+  </si>
+  <si>
+    <t>-I args</t>
+  </si>
+  <si>
+    <t>-sf args</t>
+  </si>
+  <si>
+    <t>Disabled</t>
+  </si>
+  <si>
+    <t>Set to true if needed.</t>
+  </si>
+  <si>
+    <t>Include this option in command line to enable it if needed.</t>
+  </si>
+  <si>
+    <t>Write the discovered sources and sinks to the log output. **Note: This option seems like no effect with FlowDroid that is under development.**</t>
+  </si>
+  <si>
+    <t>*UNKNOWN*</t>
+  </si>
+  <si>
+    <t>Limit the maximum number of threads to the given value. **Note: Cannot locate the effect of this option in the source code.**</t>
+  </si>
+  <si>
+    <t>100</t>
+  </si>
+  <si>
+    <t>Unlimited (-1)</t>
+  </si>
+  <si>
+    <t>Set it to the file with ICC model.</t>
+  </si>
+  <si>
+    <t>AUTO</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>CONTEXTSENSITIVE</t>
+  </si>
+  <si>
+    <t>DEFAULT</t>
+  </si>
+  <si>
+    <t>CONTEXTFLOWSENSITIVE</t>
+  </si>
+  <si>
+    <t>FLOWSENSITIVE</t>
+  </si>
+  <si>
+    <t>PROPAGATECONSTS</t>
+  </si>
+  <si>
+    <t>Disabled (StaticFieldTrackingMode is ContextFlowSensitive)</t>
+  </si>
+  <si>
+    <t>Callgraph algorithm to use (AUTO, CHA, VTA, RTA, SPARK, GEOM). **Note: AUTO and SPARK: Use Soot Pointer Anlysis Research Kit (Spark) that refines the results of CHA to achieve a more precise points-to analysis; CHA: Class Hierarychy Analysis, the fatest call graph generation mechanism, but it leads to several edges to different method definitions of subtypes; VTA: Variable-Type Analysis, with a flow-insensitive analysis; RTA: Rapid Type Anlysis, CHA with addition information about the instantiated classes; GEOM: geomPTA, a context senstitive points-to analysis based on Spark.**</t>
+  </si>
+  <si>
+    <t>PWD</t>
+  </si>
+  <si>
+    <t>Mode for considerung layout controls as sources (NONE, PWD, ALL). **Note: PWD: MatchSensitiveOnly, only use sensitive alyout components (e.g. password fields) as sources; ALL: MatchAll, use all layout components as sources.</t>
+  </si>
+  <si>
+    <t>Use the specified aliasing algorithm (NONE, FLOWSENSITIVE, PTSBASED, LAZY). **Note: FLOWSENSITIVE: A fully flow-sensitive algorithm based on Andromeda; PTSBASED: A flow-insensitive algorithm based on Soot's points-to sets; LAZY: Propagate every taint everywhere to on-demand check whether it aliases with any value access.**</t>
+  </si>
+  <si>
+    <t>SOURCELIST</t>
+  </si>
+  <si>
+    <t>Use the specified mode for defining which callbacks introduce which sources (NONE, ALL, SOURCELIST). **Note: ALL: All callback parameters are sources; SOURCELIST: Only parameters from callback methods explicitly defined as sources are treated as sources.**</t>
+  </si>
+  <si>
+    <t>Use the specified mode for reconstructing taint propagation paths (NONE, FAST, PRECISE). **Note: FAST: Reconstruct the path between source and sink, but allow for simplifications to improve performance; PRECISE: Reconstruct the precise path between source and sink, do not simplify anything.**</t>
+  </si>
+  <si>
+    <t>Use the specified mode when processing implicit data flows (NONE, ARRAYONLY, ALL). **Note: ARRAYONLY: Create a new taint when a non-tainted array is accessed using a tainted index, but do not follow other control-flow dependencies; ALL: Follow all control flow dependencies that involve tainted data.**</t>
+  </si>
+  <si>
+    <t>Use the specified code elimination algorithm (NONE, PROPAGATECONSTS, REMOVECODE). **Note: PROPAGATECONSTS: Perform an inter-procedural constant propagation and folding and then remove all code that is unreachable; REMOVECODE: in addition to the inter-procedural constant propagation and folding, also remove live code that cannot potentially influence the outcome of the taint analysis.**</t>
+  </si>
+  <si>
+    <t>Use the specified mode when tracking static data flows (CONTEXTFLOWSENSITIVE, CONTEXTFLOWINSENSITIVE, NONE). **Note: CONTEXTFLOWSENSITIVE: Track taints on static fields as normal taint abstraction, which is context- and flow-sensitive; CONTEXTFLOWINSENSITIVE: Track taints on static fields as field-based annotations, which is neitherr context-, nor flow-sensitive.**</t>
   </si>
 </sst>
 </file>
@@ -374,9 +560,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -693,557 +884,814 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25F8B51D-63B4-4281-9696-1864CD20A3E6}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="27" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="107.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="220" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="96.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="58.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="220" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C2" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
-      <c r="D5" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D7" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
-        <v>66</v>
-      </c>
-      <c r="D8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="C9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" t="s">
         <v>12</v>
       </c>
-      <c r="C10" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B11" t="s">
         <v>13</v>
       </c>
-      <c r="C11" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" t="s">
         <v>14</v>
       </c>
-      <c r="C12" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B14" t="s">
         <v>16</v>
       </c>
-      <c r="C14" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="C15" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>74</v>
+      <c r="C16" s="2" t="s">
+        <v>112</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="E16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F16" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B17" t="s">
         <v>19</v>
       </c>
-      <c r="C17" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="E17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F17" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B18" t="s">
         <v>20</v>
       </c>
-      <c r="C18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B19" t="s">
         <v>21</v>
       </c>
-      <c r="C19" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B20" t="s">
         <v>22</v>
       </c>
-      <c r="C20" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21" t="s">
         <v>23</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F21" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B22" t="s">
         <v>25</v>
       </c>
-      <c r="C22" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F22" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B23" t="s">
         <v>26</v>
       </c>
-      <c r="C23" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" t="s">
         <v>27</v>
       </c>
-      <c r="C24" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B25" t="s">
         <v>28</v>
       </c>
-      <c r="C25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="C26" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C26" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
-      <c r="C27" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C27" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B28" t="s">
         <v>31</v>
       </c>
-      <c r="C28" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C28" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B29" t="s">
         <v>32</v>
       </c>
-      <c r="C29" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" t="s">
         <v>33</v>
       </c>
-      <c r="C30" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C30" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B31" t="s">
         <v>34</v>
       </c>
-      <c r="C31" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C31" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F31" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B32" t="s">
         <v>35</v>
       </c>
-      <c r="C32" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B33" t="s">
         <v>36</v>
       </c>
-      <c r="C33" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="F33" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B34" t="s">
         <v>37</v>
       </c>
-      <c r="C34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B35" t="s">
         <v>38</v>
       </c>
-      <c r="C35" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
-      <c r="C36" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B37" t="s">
         <v>40</v>
       </c>
-      <c r="C37" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" t="s">
         <v>41</v>
       </c>
-      <c r="C38" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B39" t="s">
         <v>42</v>
       </c>
-      <c r="C39" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B40" t="s">
         <v>43</v>
       </c>
-      <c r="C40" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B41" t="s">
         <v>44</v>
       </c>
-      <c r="C41" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B42" t="s">
         <v>45</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>52</v>
+      </c>
+      <c r="B43" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>53</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="C43" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44" t="s">
         <v>47</v>
       </c>
-      <c r="C43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>52</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="C44" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>51</v>
+      </c>
+      <c r="B45" t="s">
         <v>48</v>
       </c>
-      <c r="C44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45" t="s">
-        <v>49</v>
-      </c>
-      <c r="C45" t="s">
-        <v>101</v>
+      <c r="C45" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E45" xr:uid="{10A6898C-78A3-485E-B25C-867B68744F8C}"/>
+  <autoFilter ref="A1:F45" xr:uid="{10A6898C-78A3-485E-B25C-867B68744F8C}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>